<commit_message>
necesidades excel file fixes
</commit_message>
<xml_diff>
--- a/necesidades.xlsx
+++ b/necesidades.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="vsPlJCSo2sy+oELHD/ZS2aAdQpwR8UJwCWsMS4Z68wA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="LP4gwzmpmy3FqvTSQr+rkK1+mNDUi29rL3+uZKhb7kU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
   <si>
     <t>#</t>
   </si>
@@ -43,50 +43,42 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Fundamental&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir mejorar la implicación del equipo y rendimiento, tanto a nivel individual como colectivo&lt;/b&gt;.&lt;/p&gt;
-&lt;p&gt;No es un camino fácil. De hecho, la mayoría de los titulares y gerentes de farmacia están batallando con sus equipos porque no consiguen dar con la tecla del cambio.&lt;/p&gt;
-&lt;p&gt;Lo que debes entender en este nivel es que, en vez de intentar cambiar al equipo, primero deberías cambiar tú.&lt;/p&gt;
-&lt;p&gt;Debes convertirte en el tipo de líder que consigue que su equipo le siga, no porque se sienten obligados, sino porque se creen a su líder. Debes desarrollar tus habilidades de liderazgo y comunicación, porque eso es lo que te permitirá "activar" a tu equipo.&lt;/p&gt;
-&lt;p&gt;Tener un equipo implicado y de alto rendimiento es &lt;b&gt;VITAL&lt;/b&gt; para el éxito futuro de la farmacia, porque es el &lt;b&gt;PILAR&lt;/b&gt; sobre el que se construye el resto de la Pirámide (lo básico, lo avanzado y lo diferencial).&lt;/p&gt;
-&lt;p&gt;Si esta base &lt;b&gt;NO&lt;/b&gt; es estable, podrás seguir trabajando cosas de otros niveles, pero te costará mucho hacer realidad las mejoras y lo más seguro es que, a los pocos días, el equipo vuelva a hacer lo mismo de antes.&lt;/p&gt;
+&lt;p&gt;No es un camino fácil. &lt;/p&gt; 
+&lt;p&gt;De hecho, la mayoría de los titulares y gerentes de farmacia se quedan atascados años porque NO consiguen dar con la tecla para movilizar al equipo.&lt;/p&gt;
+&lt;p&gt;Lo que debes entender en este nivel es que, en vez de intentar cambiar al equipo, &lt;b&gt;primero deberías cambiar tú&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;Debes convertirte en el tipo de líder que consigue que su equipo le siga, no porque se sienten obligados, sino porque creen en la persona que está al frente del proyecto. Sólo así podrás "activar" a tu equipo.&lt;/p&gt;
+&lt;p&gt;Tener un equipo implicado y de alto rendimiento es &lt;b&gt;VITAL&lt;/b&gt; para el éxito futuro de la farmacia, porque es el &lt;b&gt;PILAR&lt;/b&gt; sobre el que se construye el resto de la Pirámide de la Experienica (lo básico, lo avanzado y lo diferencial).&lt;/p&gt;
+&lt;p&gt;Si este pilar es débil, &lt;b&gt;NO&lt;/b&gt; soportará el trabajo que hagas en otros niveles y, no importa los cambios que intentes, a los pocos días el equipo volverá a hacer lo mismo de siempre (¿Te suena?).&lt;/p&gt;
 &lt;p&gt;Cuando aprendas cómo trabajar de la manera correcta este nivel, podrás lograr con tu farmacia &lt;b&gt;CUALQUIER COSA QUE TE PROPONGAS&lt;/b&gt;.&lt;/p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es que &lt;b&gt;mejorares tus &lt;i&gt;habilidades de liderazgo y comunicación&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Liderazgo y comunicación
 </t>
   </si>
   <si>
     <t>¿Tienes las habilidades de liderazgo necesarias para inspirar, motivar y hacer que el  equipo te siga y hagan realidad los nuevos proyectos e iniciativas que propones y de forma permanente?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Desarrollar habilidades de liderazgo y comunicación&lt;/b&gt; es lo MÁS IMPORTANTE que puedes hacer por tu farmacia.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es que &lt;b&gt;mejorares tus &lt;i&gt;habilidades de liderazgo y comunicación&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Desarrollar habilidades de liderazgo y comunicación&lt;/b&gt; es lo MÁS IMPORTANTE que puedes hacer por tu farmacia.&lt;/p&gt; 
 &lt;p&gt;&lt;b&gt;Todo está conectado:&lt;/b&gt; la rentabilidad de la farmacia y tus habilidades de liderazgo. &lt;/p&gt; 
 &lt;p&gt;Si sabes liderar de la manera correcta, &lt;b&gt;tu equipo estará más implicado&lt;/b&gt; y hará mejor su trabajo de cara al cliente. Entonces, cuando el cliente os visite, vivirá una mejor experiencia y estará &lt;b&gt;MÁS ABIERTO&lt;/b&gt; a volver a la farmacia y recomendarla a otras personas.&lt;/p&gt; &lt;p&gt;Esto hará que más personas os visiten y, como consecuencia, &lt;b&gt;la farmacia CRECERÁ.&lt;/b&gt;&lt;/p&gt;
 &lt;p&gt;&lt;i&gt;*Si quieres entender y dominar todo esto, &lt;u&gt;no olvides llegar hasta el final de la página&lt;/u&gt;&lt;/i&gt;.&lt;/p&gt;
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;A partir de mañana, dedica 10 minutos al inicio del día para comunicar los objetivos diarios y escuchar a tu equipo.&lt;/b&gt; Esta práctica no solo establece claridad en las metas, sino que también refuerza la comunicación y el compromiso del equipo. Según un estudio de &lt;i&gt;Harvard Business Review&lt;/i&gt;, equipos que reciben una comunicación diaria efectiva tienen un 30% más de probabilidad de cumplir sus objetivos.&lt;/p&gt; &lt;p&gt;Esto mejorará la implicación y motivación, creando un ambiente de trabajo más cohesionado y productivo. Mantener a todos informados fortalece el liderazgo y la comunicación efectiva en la farmacia.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;A partir de mañana, dedica 10 minutos al inicio del día para comunicar los objetivos diarios y escuchar a tu equipo.&lt;/b&gt; Esta práctica no solo establece claridad en las metas, sino que también refuerza la comunicación y el compromiso del equipo. Según un estudio de &lt;i&gt;Harvard Business Review&lt;/i&gt;, equipos que reciben una comunicación diaria efectiva tienen un 30% más de probabilidad de cumplir sus objetivos.&lt;/p&gt; &lt;p&gt;Esto mejorará la implicación y motivación, creando un ambiente de trabajo más cohesionado y productivo. Mantener a todos informados fortalece el liderazgo y la comunicación efectiva en la farmacia.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Fundamental&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir mejorar la implicación del equipo y rendimiento, tanto a nivel individual como colectivo&lt;/b&gt;.&lt;/p&gt;
-&lt;p&gt;No es un camino fácil. De hecho, la mayoría de los titulares y gerentes de farmacia están batallando con sus equipos porque no consiguen dar con la tecla del cambio.&lt;/p&gt;
-&lt;p&gt;Lo que debes entender en este nivel es que, en vez de intentar cambiar al equipo, primero deberías cambiar tú.&lt;/p&gt;
-&lt;p&gt;Debes convertirte en el tipo de líder que consigue que su equipo le siga, no porque se sienten obligados, sino porque se creen a su líder. Debes desarrollar tus habilidades de liderazgo y comunicación, porque eso es lo que te permitirá "activar" a tu equipo.&lt;/p&gt;
-&lt;p&gt;Tener un equipo implicado y de alto rendimiento es &lt;b&gt;VITAL&lt;/b&gt; para el éxito futuro de la farmacia, porque es el &lt;b&gt;PILAR&lt;/b&gt; sobre el que se construye el resto de la Pirámide (lo básico, lo avanzado y lo diferencial).&lt;/p&gt;
-&lt;p&gt;Si esta base &lt;b&gt;NO&lt;/b&gt; es estable, podrás seguir trabajando cosas de otros niveles, pero te costará mucho hacer realidad las mejoras y lo más seguro es que, a los pocos días, el equipo vuelva a hacer lo mismo de antes.&lt;/p&gt;
-&lt;p&gt;Cuando aprendas cómo trabajar de la manera correcta este nivel, podrás lograr con tu farmacia &lt;b&gt;CUALQUIER COSA QUE TE PROPONGAS&lt;/b&gt;.&lt;/p&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;coordinación del equipo&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Coordinación del equipo</t>
   </si>
   <si>
     <t>¿Tenéis algún tipo de herramienta semanal, como reuniones, que permita que el equipo colabore y se autoorganice para responder a los distintos retos que aparecen?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Muchas farmacias están lidiando con el reto de que el equipo NO es un EQUIPO, sino &lt;i&gt;un grupo de personas que trabajan juntas&lt;/i&gt;. &lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;coordinación del equipo&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;Muchas farmacias están lidiando con el reto de que el equipo NO es un EQUIPO, sino &lt;i&gt;un grupo de personas que trabajan juntas&lt;/i&gt;. &lt;/p&gt;
 &lt;p&gt;Según un estudio de McKinsey &amp; Company, la cohesión y coordinación del equipo pueden incrementar &lt;b&gt;la efectividad en un 25%&lt;/b&gt;. Para crear sentimiento de EQUIPO, necesitas incorporar dinámicas que fomenten &lt;b&gt;el sentido de pertenencia y dirección o propósito&lt;/b&gt;. &lt;/p&gt;
 &lt;p&gt;Pero lograr que tu equipo se sienta como un equipo es solo una parte; la otra está en que trabajen como un equipo. &lt;/p&gt;
 &lt;p&gt;NO importa el proyecto que sea, si no consigues coordinar a tu equipo, no lo lograrás. &lt;/p&gt;
@@ -95,18 +87,19 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige cada semana un aspecto importante para trabajar con el equipo y organiza una breve reunión para definir tareas y objetivos.&lt;/b&gt; Esto fomenta un sentido de pertenencia y mejora la coordinación. La &lt;i&gt;Universidad de Stanford&lt;/i&gt; señala que reuniones breves y efectivas pueden aumentar la productividad del equipo en un 25%.&lt;/p&gt; &lt;p&gt;Haz seguimiento al final de la semana para evaluar los logros y establecer nuevos objetivos. Saber en qué están trabajando sus compañeros permitirá al equipo apoyarse mutuamente y trabajar de manera más eficiente y armoniosa.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige cada semana un aspecto importante para trabajar con el equipo y organiza una breve reunión para definir tareas y objetivos.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Esto fomenta un sentido de pertenencia y mejora la coordinación. La &lt;i&gt;Universidad de Stanford&lt;/i&gt; señala que reuniones breves y efectivas pueden aumentar la productividad del equipo en un 25%.&lt;/p&gt; &lt;p&gt;Haz seguimiento al final de la semana para evaluar los logros y establecer nuevos objetivos. Saber en qué están trabajando sus compañeros permitirá al equipo apoyarse mutuamente y trabajar de manera más eficiente y armoniosa.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;calidad y los procesos&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Calidad y los procesos
 </t>
   </si>
   <si>
     <t>¿Tenéis procesos eficientes, digitalzaidos, que todos en el equipo conocen y siguen y donde no hay cuellos de botellas ni ralentizaciones?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Todos queremos aumentar los márgenes o el ticket medio de los clientes, pero a menudo descuidamos la &lt;b&gt;calidad y los procesos internos&lt;/b&gt;. &lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;calidad y los procesos&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;Todos queremos aumentar los márgenes o el ticket medio de los clientes, pero a menudo descuidamos la &lt;b&gt;calidad y los procesos internos&lt;/b&gt;. &lt;/p&gt;
 &lt;p&gt;Un estudio de la &lt;i&gt;Universidad de Stanford&lt;/i&gt; revela que la optimización de procesos puede &lt;b&gt;mejorar la eficiencia en un 30%&lt;/b&gt; sin necesidad de grandes inversiones. &lt;/p&gt;
 &lt;p&gt;Sin necesidad de abrir nuevos frentes, en los procesos internos podemos encontrar grandes márgenes simplemente haciendo las cosas que ya hacemos, mejor o de manera más eficiente. &lt;/p&gt;
 &lt;p&gt;Piensa en los encargos: quizás sepáis hacer encargos, pero lo hacéis en un cuaderno o sin apuntar los datos de contacto de la persona. O tal vez tenéis todo lo anterior, pero podéis mejorar el sistema de recordatorios para que no os dejen los productos colgados… &lt;/p&gt;
@@ -115,17 +108,17 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;Selecciona un proceso interno para mejorar y solicita a un miembro del equipo que cree un checklist sencillo.&lt;/b&gt; Implementar y seguir estos checklists puede reducir errores y mejorar la eficiencia, como demuestra un estudio de &lt;i&gt;McKinsey &amp; Company&lt;/i&gt;, que encontró una mejora del 20% en la eficiencia operativa con la implementación de procesos estandarizados.&lt;/p&gt; &lt;p&gt;Comparte el checklist con el equipo y realiza un seguimiento para evaluar las mejoras. Esto permitirá una operación más fluida y un servicio al cliente más consistente.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;Selecciona un proceso interno para mejorar y solicita a un miembro del equipo que cree un checklist sencillo.&lt;/b&gt;&lt;/p&gt; &lt;p&gt;Implementar y seguir estos checklists puede reducir errores y mejorar la eficiencia, como demuestra un estudio de &lt;i&gt;McKinsey &amp; Company&lt;/i&gt;, que encontró una mejora del 20% en la eficiencia operativa con la implementación de procesos estandarizados.&lt;/p&gt; &lt;p&gt;Comparte el checklist con el equipo y realiza un seguimiento para evaluar las mejoras. Esto permitirá realizar los procesos de manera más fluida y tener un servicio al cliente más consistente.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar el &lt;i&gt;rendimiento individual de cada miembro del equipo&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Rendimiento individual</t>
   </si>
   <si>
     <t>¿Sabes cómo hacer que cada miembro del equipo mejore su rendimiento individual y encuentre su mejor versión y lo estás consiguiendo?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;El rendimiento colectivo del equipo se fundamenta en buenos rendimientos individuales. &lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar el &lt;i&gt;rendimiento individual de cada miembro del equipo&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;El rendimiento colectivo del equipo se fundamenta en buenos rendimientos individuales. &lt;/p&gt;
 &lt;p&gt;Un informe de Gallup muestra que los equipos con un enfoque en el rendimiento individual son &lt;b&gt;un 21% más productivos&lt;/b&gt;. &lt;/p&gt;
 &lt;p&gt;Un equipo puede estar logrando un rendimiento y unos resultados satisfactorios, pero si se consigue activar y potenciar el rendimiento individual, el rendimiento global se disparará. &lt;/p&gt;
 &lt;p&gt;Saber &lt;b&gt;encontrar la mejor versión de cada miembro del equipo&lt;/b&gt; a nivel individual, teniendo en cuenta sus puntos fuertes y débiles, es &lt;b&gt;VITAL&lt;/b&gt; para cualquier farmacia que aspire a más.&lt;/p&gt;
@@ -133,16 +126,16 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;Proporciona feedback positivo específico a cada miembro del equipo.&lt;/b&gt; Reconocer logros individuales no solo motiva, sino que también mejora el rendimiento general. Según &lt;i&gt;Gallup&lt;/i&gt;, el reconocimiento efectivo puede aumentar la productividad de los empleados en un 30%.&lt;/p&gt; &lt;p&gt;Esto fomentará un ambiente de trabajo más positivo y productivo, beneficiando tanto a los trabajadores como al rendimiento global del equipo.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;Proporciona feedback positivo específico a cada miembro del equipo.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Reconocer logros individuales no solo motiva, sino que también mejora el rendimiento general. Según &lt;i&gt;Gallup&lt;/i&gt;, el reconocimiento efectivo puede aumentar la productividad de los empleados en un 30%.&lt;/p&gt; &lt;p&gt;Esto fomentará un ambiente de trabajo más positivo y productivo, beneficiando tanto a los trabajadores como al rendimiento global del equipo.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;fomentar la &lt;i&gt;autonomía y responsabilidad del equipo de farmacia&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;</t>
+    <t>Autonomía y responsabilidad</t>
   </si>
   <si>
     <t>¿Delegas todas las tareas que no son fundamentales y tu equipo las desempeña de manera autónoma  y responsable, de forma que te puedas olvidar de esas tareas y no preocuparte por ellas porque sabes que se hacen bien?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Muchos titulares y gerentes&lt;/b&gt; tienen miedo de darle responsabilidades a las personas de su equipo porque piensan que se van “quemar” o que les van a pedir más dinero.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;fomentar la &lt;i&gt;autonomía y responsabilidad del equipo de farmacia&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Muchos titulares y gerentes&lt;/b&gt; tienen miedo de darle responsabilidades a las personas de su equipo porque piensan que se van “quemar” o que les van a pedir más dinero.&lt;/p&gt; 
 &lt;p&gt;&lt;b&gt;La psicología demuestra que es ¡Justo lo contrario!&lt;/b&gt; Cuantas más tareas delegamos, más importante hacemos sentir a la otra persona, se hace más responsable y rinde mejor.&lt;/p&gt; 
 &lt;p&gt;Piensa en tu equipo, &lt;b&gt;¿acaso la persona que mejor trabaja&lt;/b&gt; no es la que más tareas y responsabilidades tiene y la que peor trabaja es la que menos tareas y responsabilidades tiene?&lt;/p&gt; 
 &lt;p&gt;&lt;b&gt;¡No es casualidad!&lt;/b&gt;&lt;/p&gt;
@@ -150,14 +143,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Proporciona feedback positivo específico a cada miembro del equipo.&lt;/b&gt; Reconocer logros individuales no solo motiva, sino que también mejora el rendimiento general. Según &lt;i&gt;Gallup&lt;/i&gt;, el reconocimiento efectivo puede aumentar la productividad de los empleados en un 30%.&lt;/p&gt; &lt;p&gt;Esto fomentará un ambiente de trabajo más positivo y productivo, beneficiando tanto a los trabajadores como al rendimiento global del equipo.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Proporciona feedback positivo específico a cada miembro del equipo.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Reconocer logros individuales no solo motiva, sino que también mejora el rendimiento general. Según &lt;i&gt;Gallup&lt;/i&gt;, el reconocimiento efectivo puede aumentar la productividad de los empleados en un 30%.&lt;/p&gt; &lt;p&gt;Esto fomentará un ambiente de trabajo más positivo y productivo, beneficiando tanto a los trabajadores como al rendimiento global del equipo.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
     <t>BASICO</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Básico&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que la experiencia de vuestros clientes y pacientes sea tan buena que quieran volver a la farmacia&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Básico&lt;/b&gt;. &lt;/p&gt;
+&lt;p&gt;En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que la experiencia de vuestros clientes y pacientes sea tan buena que quieran volver a la farmacia&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Es decir, ahora os debéis centrar en la &lt;b&gt;Fidelización de clientes y pacientes&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;El crecimiento de una farmacia en este nivel pasa por centrarse en mejorar la experiencia de los clientes que &lt;i&gt;entran&lt;/i&gt; en la farmacia. Y en este sentido, &lt;b&gt;TODO&lt;/b&gt; cuenta: lo que ve desde fuera antes de entrar, lo primero que ve, huele o escucha al entrar en la farmacia, el camino al mostrador, la persona que le atiende, el consejo que recibe, lo que vive antes de marcharse y mucho más. Cada cosa cuenta, así que, como ves, tienes mucho margen de mejora.&lt;/p&gt;
 &lt;p&gt;Piénsalo un momento. La única razón por la que la farmacia puede seguir abriendo cada día no son los seguidores de Instagram, ni los proveedores de la farmacia... Es porque los clientes siguen eligiendo vuestra farmacia día tras día. Por eso son lo &lt;b&gt;MÁS IMPORTANTE&lt;/b&gt;.&lt;/p&gt;
@@ -166,14 +160,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la calidad en la &lt;i&gt;atención farmacéutica&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Atención farmacéutica
 </t>
   </si>
   <si>
     <t xml:space="preserve">¿Todo el equipo de farmacia ofrece al cliente y paciente una atención farmacéutica orientada a sus necesidades y con una calidad similar (incluye medidas farmacológicas y no farmacológicas, beneficios del tratamiento, posología, etc.)? </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;La atención farmacéutica es el corazón de la farmacia. Todo lo que haces, desde las compras hasta las formaciones, es para llegar &lt;b&gt;LO MEJOR PREPARADO&lt;/b&gt; a este momento.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la calidad en la &lt;i&gt;atención farmacéutica&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;La atención farmacéutica es el corazón de la farmacia. Todo lo que haces, desde las compras hasta las formaciones, es para llegar &lt;b&gt;LO MEJOR PREPARADO&lt;/b&gt; a este momento.&lt;/p&gt; 
 &lt;p&gt;Un estudio de la &lt;i&gt;Organización Mundial de la Salud&lt;/i&gt; muestra que la atención farmacéutica de calidad aumenta la adherencia al tratamiento en un 40%.&lt;/p&gt;
 &lt;p&gt;Si, en el momento de tener al cliente o paciente delante, sois capaces de ayudarle y aportarle el máximo valor posible, vuestra farmacia crecerá.&lt;/p&gt; 
 &lt;p&gt;Recuerda: no hay negocio que ayude mucho a mucha gente y no gane mucho. Si quieres que tu farmacia crezca, céntrate en &lt;b&gt;AYUDAR&lt;/b&gt; mediante la atención farmacéutica.&lt;/p&gt;
@@ -181,18 +176,19 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Incorpora una medida higiénico-dietética en el consejo farmacéutico sobre la patología del cliente.&lt;/b&gt; Ofrecer un consejo integral y personalizado puede aumentar la satisfacción del cliente. Un estudio de la &lt;i&gt;Universidad de Harvard&lt;/i&gt; muestra que un enfoque integral en la atención puede mejorar la adherencia al tratamiento en un 40%.&lt;/p&gt; &lt;p&gt;Esto fortalecerá la lealtad del cliente a la farmacia y mejorará la calidad de la atención ofrecida.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Incorpora una medida higiénico-dietética en el consejo farmacéutico sobre la patología del cliente.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Ofrecer un consejo integral y personalizado puede aumentar la satisfacción del cliente. Un estudio de la &lt;i&gt;Universidad de Harvard&lt;/i&gt; muestra que un enfoque integral en la atención puede mejorar la adherencia al tratamiento en un 40%.&lt;/p&gt; &lt;p&gt;Esto fortalecerá la lealtad del cliente a la farmacia y mejorará la calidad de la atención ofrecida.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;identificación de clientes y pacientes&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Identificación de clientes y pacientes
 </t>
   </si>
   <si>
     <t>¿Se están  registrando y asociando al menos el 80% de las transacciones diarias en el mostrador (medicamentos y venta libre) a perfiles de pacientes en el software de la farmacia para mejorar la personalización en el futuro?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Es &lt;b&gt;IMPOSIBLE&lt;/b&gt; personalizar la experiencia de los clientes sin información.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;identificación de clientes y pacientes&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;Es &lt;b&gt;IMPOSIBLE&lt;/b&gt; personalizar la experiencia de los clientes sin información.&lt;/p&gt;
 &lt;p&gt;Un estudio de &lt;i&gt;Deloitte&lt;/i&gt; revela que las empresas que personalizan la experiencia del cliente tienen un 60% más de probabilidades de ser elegidas por encima de la competencia.&lt;/p&gt;
 &lt;p&gt;El gran problema en la mayoría de farmacias es que el 90% de las transacciones son anónimas.&lt;/p&gt;
 &lt;p&gt;Por eso, es &lt;b&gt;TAN IMPORTANTE&lt;/b&gt; que empecéis a identificar todas las transacciones, tanto de venta libre como de medicamentos.&lt;/p&gt;
@@ -201,17 +197,18 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;Empieza a pedir el nombre y un dato de contacto en cada transacción.&lt;/b&gt; Esta práctica te permitirá personalizar la experiencia y mejorar la relación con los clientes. Según &lt;i&gt;Deloitte&lt;/i&gt;, las empresas que personalizan la experiencia del cliente tienen un 60% más de probabilidad de ser elegidas por encima de la competencia.&lt;/p&gt; &lt;p&gt;Facilitará la implementación de estrategias de marketing más efectivas y personalizadas.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;Empieza a pedir el nombre y un dato de contacto en cada transacción.&lt;/b&gt; Esta práctica te permitirá personalizar la experiencia y mejorar la relación con los clientes. Según &lt;i&gt;Deloitte&lt;/i&gt;, las empresas que personalizan la experiencia del cliente tienen un 60% más de probabilidad de ser elegidas por encima de la competencia.&lt;/p&gt; &lt;p&gt;Facilitará la implementación de estrategias de marketing más efectivas y personalizadas.&lt;/p&gt;&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;comunicación y el seguimiento&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Comunicación y el seguimiento
 </t>
   </si>
   <si>
     <t>¿Ofrecéis a los clientes y pacientes que visitan a la farmacia diferentes canales de comunicación, incluyendo medios digitales (por ejemplo, WhatsApp) y se fomenta el uso por parte de ellos para mantener una relación más estrecha?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En el siglo pasado, el radio de acción de una farmacia se limitaba a las visitas del paciente.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;comunicación y el seguimiento&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;En el siglo pasado, el radio de acción de una farmacia se limitaba a las visitas del paciente.&lt;/p&gt; 
 &lt;p&gt;Podíais estar cerca de ellos sólo cuando os visitaban o llamaban por teléfono.&lt;/p&gt; 
 &lt;p&gt;Ahora, la tecnología ha cambiado todo esto. Es posible estar cerca del cliente también cuando no está en la farmacia, usando, por ejemplo, &lt;i&gt;WhatsApp Business&lt;/i&gt;.&lt;/p&gt; 
 &lt;p&gt;Un estudio de &lt;i&gt;Accenture&lt;/i&gt; muestra que el 70% de los consumidores prefieren interactuar con las empresas a través de mensajes de texto.&lt;/p&gt;
@@ -220,21 +217,20 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Compra un número e instala WhatsApp Business (y WhatsApp Business Web en un ordenador). &lt;/p&gt;
+    <t>&lt;p&gt;Compra un número e instala WhatsApp Business (y WhatsApp Business Web en un ordenador). &lt;/p&gt;
 &lt;p&gt;Si ya lo tienes, crea un sistema para que los mensajes se respondan &lt;b&gt;antes de 1 hora&lt;/b&gt;. Esto te permitirá mantener un contacto más cercano y rápido con tus clientes, mejorando su experiencia y la percepción de tu servicio. &lt;/p&gt; 
 &lt;p&gt;La respuesta rápida fortalecerá la relación con el cliente y su confianza en tu farmacia.&lt;/p&gt;
-&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
-</t>
+&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar o potenciar los &lt;i&gt;servicios relacionados con la salud que ofrecéis&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Servicios relacionados con la salud</t>
   </si>
   <si>
     <t>¿Ofrecéis servicios relacionados con salud que incluyen, además de mediciones, un registro histórico de las consultas y seguimiento farmacoterapeútico?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En un contexto donde todas las farmacias venden los mismos productos, los servicios son clave para diferenciarse.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar o potenciar los &lt;i&gt;servicios relacionados con la salud que ofrecéis&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;En un contexto donde todas las farmacias venden los mismos productos, los servicios son clave para diferenciarse.&lt;/p&gt;
 &lt;p&gt;Un informe de &lt;i&gt;Bain &amp; Company&lt;/i&gt; indica que las empresas que ofrecen servicios diferenciados tienen un 25% más de retención de clientes.&lt;/p&gt;
 &lt;p&gt;En muchas farmacias, se piensa que tener un cartel en la puerta es tener un servicio. O creen que un servicio es simplemente poner una mesa y un tensiómetro.&lt;/p&gt;
 &lt;p&gt;Cuando hablamos de servicios aquí, hablamos de tener servicios profesionalizados, con mediciones, seguimiento y consejo experto.&lt;/p&gt;
@@ -248,11 +244,12 @@
 &lt;p&gt;Según un informe de &lt;i&gt;McKinsey&lt;/i&gt;, las farmacias que mejoran la calidad de sus servicios pueden aumentar la satisfacción del cliente en un 30%.&lt;/p&gt;
 &lt;p&gt;Por ejemplo, si no estás midiendo tus servicios, comienza a hacerlo. Si ya los mides, empieza a registrar los datos para tener un histórico de mediciones. Y ya los registras, haz seguimiento a los pacientes en su próxima visita y muéstrales visualmente (por ejemplo, con una gráfica) cómo está mejorando gracias al servicio que le estáis ofreciendo. &lt;/p&gt; 
 &lt;p&gt;Esto diferenciará tu farmacia y aumentará la satisfacción y fidelidad del cliente.&lt;/p&gt; 
-&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Básico&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que la experiencia de vuestros clientes y pacientes sea tan buena que quieran volver a la farmacia&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Básico&lt;/b&gt;. &lt;/p&gt;
+&lt;p&gt;En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que la experiencia de vuestros clientes y pacientes sea tan buena que quieran volver a la farmacia&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Es decir, ahora os debéis centrar en la &lt;b&gt;Fidelización de clientes y pacientes&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;El crecimiento de una farmacia en este nivel pasa por centrarse en mejorar la experiencia de los clientes que &lt;i&gt;entran&lt;/i&gt; en la farmacia. Y en este sentido, &lt;b&gt;TODO&lt;/b&gt; cuenta: lo que ve desde fuera antes de entrar, lo primero que ve, huele o escucha al entrar en la farmacia, el camino al mostrador, la persona que le atiende, el consejo que recibe, lo que vive antes de marcharse y mucho más. Cada cosa cuenta, así que, como ves, tienes mucho margen de mejora.&lt;/p&gt;
 &lt;p&gt;Piénsalo un momento. La única razón por la que la farmacia puede seguir abriendo cada día no son los seguidores de Instagram, ni los proveedores de la farmacia... Es porque los clientes siguen eligiendo vuestra farmacia día tras día. Por eso son lo &lt;b&gt;MÁS IMPORTANTE&lt;/b&gt;.&lt;/p&gt;
@@ -261,13 +258,13 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;experiencia de compra de los clientes y pacientes&lt;/i&gt; que os visitan&lt;/b&gt;.&lt;/p&gt;</t>
+    <t>Experiencia de compra</t>
   </si>
   <si>
     <t xml:space="preserve">¿Has creado un ambiente agradable y acogedor en tu farmacia, que va más allá de  la limpieza y la organización, incluyendo detalles como una agradable fragancia, música ambiental, una zona de espera cómoda y otros servicios adicionales? </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;La experiencia del cliente incluye muchos factores que afectan la impresión que damos.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;experiencia de compra de los clientes y pacientes&lt;/i&gt; que os visitan&lt;/b&gt;.&lt;/p&gt;&lt;p&gt;La experiencia del cliente incluye muchos factores que afectan la impresión que damos.&lt;/p&gt;
 &lt;p&gt;Según un estudio de &lt;i&gt;PWC&lt;/i&gt;, el 73% de los consumidores afirma que la experiencia de compra es un factor clave en sus decisiones de compra.&lt;/p&gt;
 &lt;p&gt;Dentro de esos factores está la farmacia como espacio físico y si la experiencia de compra es agradable.&lt;/p&gt;
 &lt;p&gt;Esto no sumará directamente a las ventas, pero sí a mejorar la experiencia general.&lt;/p&gt;
@@ -277,13 +274,14 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;Reorganiza una categoría de productos para mejorar la disposición y visibilidad.&lt;/b&gt; Un estudio de &lt;i&gt;Forrester&lt;/i&gt; muestra que una buena disposición en el punto de venta puede aumentar las ventas en un 20%.&lt;/p&gt; &lt;p&gt;Asegúrate de que todos los productos estén bien colocados, con precios visibles y una categoría claramente señalizada. Una presentación clara y ordenada mejora la percepción del cliente y facilita la compra.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;Reorganiza una categoría de productos para mejorar la disposición y visibilidad.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Un estudio de &lt;i&gt;Forrester&lt;/i&gt; muestra que una buena disposición en el punto de venta puede aumentar las ventas en un 20%.&lt;/p&gt; &lt;p&gt;Asegúrate de que todos los productos estén bien colocados, con precios visibles y una categoría claramente señalizada. Una presentación clara y ordenada mejora la percepción del cliente y facilita la compra.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
     <t>AVANZADO</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Avanzado&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir estar cerca de vuestros clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando no están&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Avanzado&lt;/b&gt;. &lt;/p&gt;
+&lt;p&gt;En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir estar cerca de vuestros clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando no están&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Y la forma de lograrlo es mediante el uso &lt;i&gt;correcto&lt;/i&gt; de la Digitalización.&lt;/p&gt;
 &lt;p&gt;Antes de seguir, quiero darte la enhorabuena. Estás en un nivel donde cada vez vas abriendo una brecha más grande entre las farmacias “normales y corrientes” y la tuya. Ahora no puedes seguir al "rebaño" porque habéis avanzado hasta un punto donde tenéis la responsabilidad de innovar.&lt;/p&gt;
 &lt;p&gt;Y aquí es necesario hablar del uso de la tecnología con una finalidad muy clara: estar cerca y acompañar a los clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando están fuera de ella.&lt;/p&gt;
@@ -292,14 +290,14 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;implementar o potenciar la &lt;i&gt;teleasistencia&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Teleasistencia</t>
   </si>
   <si>
     <t>¿Ofrecéis un soporte al cliente ágil y eficiente con respuesta en menos de 2 horas a través de medios digitales (por ejemplo, con WhatsApp u otra aplicación) para que puedan preguntaros sus dudas sobre su salud y los productos farmacéuticos?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;La tecnología y los teléfonos inteligentes han cambiado nuestras vidas a todos los niveles, también a nivel sanitario.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;implementar o potenciar la &lt;i&gt;teleasistencia&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;La tecnología y los teléfonos inteligentes han cambiado nuestras vidas a todos los niveles, también a nivel sanitario.&lt;/p&gt;
 &lt;p&gt;Especialmente desde el Covid, cuando nos vimos forzados a hacer todo de manera digital.&lt;/p&gt;
 &lt;p&gt;En la farmacia, todas estas tendencias tienen un nombre propio: &lt;i&gt;WhatsApp&lt;/i&gt;.&lt;/p&gt; 
 &lt;p&gt;Un informe de &lt;i&gt;Statista&lt;/i&gt; muestra que el 67% de los consumidores prefieren usar &lt;i&gt;WhatsApp&lt;/i&gt; para comunicarse con empresas.&lt;/p&gt;
@@ -313,11 +311,12 @@
 &lt;p&gt;Esto proporcionará valor añadido y fortalecerá la relación con tus clientes, demostrando un cuidado proactivo. &lt;/p&gt;
 &lt;p&gt;Según &lt;i&gt;PWC&lt;/i&gt;, el 73% de los consumidores valoran la información adicional como parte del servicio.&lt;/p&gt;
 &lt;p&gt;Al ofrecer información relevante, posicionarás tu farmacia como una fuente confiable de consejo y apoyo.&lt;/p&gt;
-&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Avanzado&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir estar cerca de vuestros clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando no están&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Avanzado&lt;/b&gt;. &lt;/p&gt;
+&lt;p&gt;En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir estar cerca de vuestros clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando no están&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Y la forma de lograrlo es mediante el uso &lt;i&gt;correcto&lt;/i&gt; de la Digitalización.&lt;/p&gt;
 &lt;p&gt;Antes de seguir, quiero darte la enhorabuena. Estás en un nivel donde cada vez vas abriendo una brecha más grande entre las farmacias “normales y corrientes” y la tuya. Ahora no puedes seguir al "rebaño" porque habéis avanzado hasta un punto donde tenéis la responsabilidad de innovar.&lt;/p&gt;
 &lt;p&gt;Y aquí es necesario hablar del uso de la tecnología con una finalidad muy clara: estar cerca y acompañar a los clientes y pacientes, no sólo cuando están dentro de la farmacia, sino también cuando están fuera de ella.&lt;/p&gt;
@@ -326,14 +325,14 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;educación sanitaria&lt;/i&gt; que dais a vuestros clientes y pacientes&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Educación sanitaria</t>
   </si>
   <si>
     <t xml:space="preserve">¿Implementáis estrategias de educación sanitaria a través de medios digitales para proporcionar regularmente a los clientes información relevante y actualizada sobre su salud y bienestar?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;La educación sanitaria es una de las 5 tareas fundamentales que la &lt;i&gt;OMS&lt;/i&gt; atribuye a las farmacias.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;educación sanitaria&lt;/i&gt; que dais a vuestros clientes y pacientes&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;La educación sanitaria es una de las 5 tareas fundamentales que la &lt;i&gt;OMS&lt;/i&gt; atribuye a las farmacias.&lt;/p&gt;
 &lt;p&gt;El problema es que hasta ahora, las posibilidades de la farmacia eran &lt;b&gt;MUY LIMITADAS&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Se hacía uno a uno en el mostrador, o se limitaba a repartir folletos.&lt;/p&gt;
 &lt;p&gt;Ahora tenemos nuevos canales de comunicación que nos permiten estar más cerca del cliente y paciente.&lt;/p&gt;
@@ -348,18 +347,19 @@
 &lt;p&gt;Un estudio de la &lt;i&gt;Universidad de Pennsylvania&lt;/i&gt; encontró que las campañas educativas personalizadas pueden aumentar la lealtad del cliente en un 25%.&lt;/p&gt; 
 &lt;p&gt;Esta segmentación mejorará la educación sanitaria y posicionará tu farmacia como un referente en salud para tus clientes.&lt;/p&gt;
 &lt;p&gt;Al mantener informados a tus clientes, fomentarás una relación de confianza y fidelidad.&lt;/p&gt; 
-&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar vuestra estrategia &lt;i&gt;marketing y las promociones&lt;/i&gt; que lleváis a cabo&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Marketing y las promociones
 </t>
   </si>
   <si>
     <t>¿Se utilizan los datos recogidos para segmentar y personalizar las campañas y servicios de acuerdo al perfil de los clientes, de sus compras pasadas y de sus preferencias e intereses?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;La única forma de que una estrategia de marketing no se convierta en spam es conociendo a los clientes.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar vuestra estrategia &lt;i&gt;marketing y las promociones&lt;/i&gt; que lleváis a cabo&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;La única forma de que una estrategia de marketing no se convierta en spam es conociendo a los clientes.&lt;/p&gt;
 &lt;p&gt;Si esta es la necesidad vital de tu farmacia, ya debes identificar al menos el 80% de las transacciones en el mostrador.&lt;/p&gt;
 &lt;p&gt;Esa información es &lt;b&gt;ORO&lt;/b&gt;. Ahora debes concentrarte en &lt;b&gt;EXPLOTAR&lt;/b&gt; esos datos de manera estratégica.&lt;/p&gt;
 &lt;p&gt;&lt;i&gt;Harvard Business School&lt;/i&gt; afirma que las campañas de marketing personalizadas tienen una tasa de conversión (ventas) un 30% superior.&lt;/p&gt;
@@ -369,23 +369,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Un estudio de &lt;i&gt;HubSpot&lt;/i&gt; muestra que el marketing personalizado tiene un 29% más de tasa de conversión.&lt;/p&gt;
+    <t>&lt;p&gt;Un estudio de &lt;i&gt;HubSpot&lt;/i&gt; muestra que el marketing personalizado tiene un 29% más de tasa de conversión.&lt;/p&gt;
 &lt;p&gt;Escoge una promoción o un servicio, filtra en el programa de gestión de la farmacia a los clientes que pueden estar interesados a partir de su historial de compras. &lt;/p&gt;
 &lt;p&gt;Cuando lo tengas, mételos en WhatsApp, crea una etiqueta para ellos y envíales una secuencia de mensajes donde el foco sea aportar valor (no vender).&lt;/p&gt;
 &lt;p&gt;Esto permitirá una comunicación directa y personalizada, aumentando la efectividad de las promociones y la satisfacción del cliente. &lt;/p&gt;
 &lt;p&gt;Un marketing dirigido y personalizado incrementará las probabilidades de éxito de tus campañas.&lt;/p&gt;
-&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
-</t>
+&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;organización de eventos&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Organización de eventos
 </t>
   </si>
   <si>
     <t>¿Organizáis eventos como talleres, cursos u otras actividades educativas ofreciendo a los clientes la oportunidad de aprender y mejorar su salud de manera interactiva y enriquecedora?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;El futuro de la farmacia no es ser solo un "dispensador de medicamentos", sino ser un AGENTE SANITARIO y un REFERENTE en salud.&lt;/b&gt; Aquí, los eventos son una pieza fundamental.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;organización de eventos&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;El futuro de la farmacia no es ser solo un "dispensador de medicamentos", sino ser un AGENTE SANITARIO y un REFERENTE en salud.&lt;/b&gt; Aquí, los eventos son una pieza fundamental.&lt;/p&gt; 
 &lt;p&gt;Un estudio de la &lt;i&gt;Universidad de Columbia&lt;/i&gt; muestra que los eventos en farmacias aumentan la lealtad del cliente en un 20%.&lt;/p&gt; 
 &lt;p&gt;Mediante la organización de charlas o talleres, puedes convertir a tu farmacia en un referente y, quién sabe, quizás nutrir un servicio o crear uno nuevo según el éxito de un evento.&lt;/p&gt; 
 &lt;p&gt;Recuerda, los eventos no tienen que ser solo presenciales; también puedes hacerlos online, especialmente si tu farmacia no va sobrada de espacio.&lt;/p&gt;
@@ -393,17 +393,18 @@
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;Invita a un experto para dar una charla y promuévela a través de WhatsApp.&lt;/b&gt; Organizar eventos educativos atraerá a más clientes y mejorará la visibilidad de tu farmacia. Según &lt;i&gt;Eventbrite&lt;/i&gt;, los eventos educativos pueden aumentar la participación de clientes en un 40%.&lt;/p&gt; &lt;p&gt;Esto fortalecerá la relación con la comunidad y atraerá a nuevos clientes.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;b&gt;Invita a un experto para dar una charla y promuévela a través de WhatsApp.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Organizar eventos educativos atraerá a más clientes y mejorará la visibilidad de tu farmacia. Según &lt;i&gt;Eventbrite&lt;/i&gt;, los eventos educativos pueden aumentar la participación de clientes en un 40%.&lt;/p&gt; &lt;p&gt;Esto fortalecerá la relación con la comunidad y atraerá a nuevos clientes.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;fortalecer la &lt;i&gt;identidad de marca de la farmacia en las RRSS&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Identidad de marca
 </t>
   </si>
   <si>
     <t xml:space="preserve">¿La farmacia tiene una identidad visual y una imagen de marca coherente y reconocible dentro de la farmacia y en todos los canales de comunicación, como el sitio web, redes sociales y materiales de marketing?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Muchas farmacias que dan el salto a las redes sociales se inspiran en otras farmacias.&lt;/b&gt; El problema es que esas farmacias se inspiraron a su vez en otras farmacias que ya estaban haciendo lo que ellas querían.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;fortalecer la &lt;i&gt;identidad de marca de la farmacia en las RRSS&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Muchas farmacias que dan el salto a las redes sociales se inspiran en otras farmacias.&lt;/b&gt; El problema es que esas farmacias se inspiraron a su vez en otras farmacias que ya estaban haciendo lo que ellas querían.&lt;/p&gt; 
 &lt;p&gt;¿Resultado? Todas las farmacias tienen una imagen y un estilo de comunicación similares.&lt;/p&gt; 
 &lt;p&gt;Según un informe de &lt;i&gt;Hootsuite&lt;/i&gt;, el 52% de los usuarios de redes sociales prefiere interactuar con marcas que tienen una identidad única.&lt;/p&gt; 
 &lt;p&gt;Si esta es tu necesidad vital, debes crear una &lt;b&gt;identidad digital&lt;/b&gt; para tu farmacia que sea propia y trasladarla a TODO lo que hagas en las redes sociales.&lt;/p&gt;
@@ -411,14 +412,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Define una guía de estilo para redes sociales con colores y recursos visuales.&lt;/b&gt; Esto creará una identidad digital consistente y profesional. Un estudio de &lt;i&gt;Sprout Social&lt;/i&gt; revela que un branding consistente puede aumentar el reconocimiento de la marca en un 33%.&lt;/p&gt; &lt;p&gt;Una imagen coherente en redes sociales atraerá a más seguidores y mejorará la percepción de tu marca.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Define una guía de estilo para redes sociales con colores y recursos visuales.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Esto creará una identidad digital consistente y profesional. Un estudio de &lt;i&gt;Sprout Social&lt;/i&gt; revela que un branding consistente puede aumentar el reconocimiento de la marca en un 33%.&lt;/p&gt; &lt;p&gt;Una imagen coherente en redes sociales atraerá a más seguidores y mejorará la percepción de tu marca.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
     <t>DIFERENCIAL</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Diferencial&lt;/b&gt;. En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que más personas entren en la farmacia o le compren por internet gracias al Marketing online&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Según el análisis de tus respuestas, el nivel de desarrollo actual de tu farmacia es el &lt;b&gt;Nivel Diferencial&lt;/b&gt;. &lt;/p&gt;
+&lt;p&gt;En este nivel, el reto más importante en que os debéis centrar es en &lt;b&gt;cómo conseguir que más personas entren en la farmacia o le compren por internet gracias al Marketing online&lt;/b&gt;.&lt;/p&gt;
 &lt;p&gt;Si tu farmacia está en este nivel, ¡Enhorabuena! Estás entre el 2% de las farmacias que &lt;b&gt;REALMENTE&lt;/b&gt; están a la vanguardia.&lt;/p&gt;
 &lt;p&gt;Mientras que en el nivel avanzado la farmacia se centra en la digitalización de la experiencia del cliente actual (el que ya ha comprado al menos una vez en la farmacia), en éste se da un salto y se empieza a enfocar también en el &lt;b&gt;cliente potencial&lt;/b&gt; (los que no conocen o no han comprado todavía en la farmacia).&lt;/p&gt;
 &lt;p&gt;En este nivel DEBES aprender a crear &lt;b&gt;EMBUDOS DE VENTA&lt;/b&gt; que conviertan a una persona que no os conoce, en un seguidor, después en un comprador y, por último, en un cliente habitual.&lt;/p&gt;
@@ -427,14 +429,15 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;presencia digital&lt;/i&gt; en todos los canales&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Presencia digital
 </t>
   </si>
   <si>
     <t xml:space="preserve">¿Tenéis una presencia digital bien orquestada, con una web, redes sociales y un perfil en Google My Business, para maximizar vuestra visibilidad y llegar a más clientes potenciales?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Muchas farmacias piensan que con tener un logo y un perfil en redes sociales es suficiente para tener una presencia digital profesional.&lt;/b&gt; Siento decirte que NO BASTA con eso.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;presencia digital&lt;/i&gt; en todos los canales&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Muchas farmacias piensan que con tener un logo y un perfil en redes sociales es suficiente para tener una presencia digital profesional.&lt;/b&gt; Siento decirte que NO BASTA con eso.&lt;/p&gt; 
 &lt;p&gt;Un estudio de &lt;i&gt;Google&lt;/i&gt; muestra que las empresas con una presencia digital sólida tienen un 70% más de probabilidades de ser consideradas por los consumidores.&lt;/p&gt; 
 &lt;p&gt;Se necesita más que eso para tener una presencia digital estable: una página web conectada a las redes sociales o un perfil de &lt;i&gt;Google My Business&lt;/i&gt; actualizado, donde cada comentario, positivo o no, tenga una respuesta.&lt;/p&gt; 
 &lt;p&gt;Cuando se hace de la manera correcta y estratégica, la farmacia empieza a jugar directamente en otra liga.&lt;/p&gt;
@@ -442,18 +445,18 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Asegúrate de que tu perfil de Google My Business esté actualizado con horarios y contactos correctos. &lt;/p&gt; &lt;p&gt;Si ya lo tienes, anima a las personas que visitan la farmacia a que os dejen un comentario positivo. Y a cada comentario que recibáis, ya sea positivo o negativo, no olvideís dejarles una respuesta.&lt;/p&gt; &lt;p&gt;Según &lt;i&gt;BrightLocal&lt;/i&gt;, las empresas que responden a los comentarios tienen un 70% más de probabilidades de atraer nuevos clientes.&lt;/p&gt;&lt;p&gt;Esta sencilla acción, te ayudará a posicionar mejor tu farmacia en Google, dará más fiabilidad a la la presencia digital de la farmacia y mejorar, en definitiva, vuestra reputación online. &lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Asegúrate de que tu perfil de Google My Business esté actualizado con horarios y contactos correctos. &lt;/p&gt; &lt;p&gt;Si ya lo tienes, anima a las personas que visitan la farmacia a que os dejen un comentario positivo. Y a cada comentario que recibáis, ya sea positivo o negativo, no olvideís dejarles una respuesta.&lt;/p&gt; &lt;p&gt;Según &lt;i&gt;BrightLocal&lt;/i&gt;, las empresas que responden a los comentarios tienen un 70% más de probabilidades de atraer nuevos clientes.&lt;/p&gt;&lt;p&gt;Esta sencilla acción, te ayudará a posicionar mejor tu farmacia en Google, dará más fiabilidad a la la presencia digital de la farmacia y mejorar, en definitiva, vuestra reputación online. &lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;aprender a desarrollar &lt;i&gt;embudos de marketing&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Embudos de marketing</t>
   </si>
   <si>
     <t xml:space="preserve">¿Tenéis una estrategia clara para convertir a los seguidores en clientes llevándolos a través de un proceso paso a paso a vuestra farmacia física, tienda online u otro canal de pago?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Estar en las redes sociales, publicar, tener una página web o un perfil en Google My Business NO SIRVE DE NADA si no tienes al menos un buen EMBUDO DE VENTAS&lt;/b&gt;.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;aprender a desarrollar &lt;i&gt;embudos de marketing&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Estar en las redes sociales, publicar, tener una página web o un perfil en Google My Business NO SIRVE DE NADA si no tienes al menos un buen EMBUDO DE VENTAS&lt;/b&gt;.&lt;/p&gt; 
 &lt;p&gt;Si tu farmacia está en este nivel, tu prioridad debe ser diseñar un proceso paso a paso que convierta a la gente que no te conoce en seguidores, en compradores, y en clientes habituales.&lt;/p&gt; 
 &lt;p&gt;Un informe de &lt;i&gt;HubSpot&lt;/i&gt; muestra que las empresas con embudos de ventas bien diseñados tienen un 60% más de conversión de leads en clientes.&lt;/p&gt; 
 &lt;p&gt;Debes crear tus propios embudos de ventas. Las farmacias que hacen esto son las que podríamos llamar &lt;b&gt;pioneras&lt;/b&gt;.&lt;/p&gt;
@@ -461,18 +464,19 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige un producto o servicio y crea una página con formulario de contacto o pasarela de compra.&lt;/b&gt; Un embudo de ventas bien diseñado facilita la conversión de visitantes en clientes. &lt;i&gt;HubSpot&lt;/i&gt; indica que un embudo de ventas optimizado puede aumentar la tasa de conversión en un 20%.&lt;/p&gt; &lt;p&gt;Esto ayudará a convertir el interés en ventas reales y aumentará las oportunidades de negocio.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige un producto o servicio y crea una página con formulario de contacto o pasarela de compra.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Un embudo de ventas bien diseñado facilita la conversión de visitantes en clientes. &lt;i&gt;HubSpot&lt;/i&gt; indica que un embudo de ventas optimizado puede aumentar la tasa de conversión en un 20%.&lt;/p&gt; &lt;p&gt;Esto ayudará a convertir el interés en ventas reales y aumentará las oportunidades de negocio.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;incrementar la &lt;i&gt;generación de tráfico&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+    <t xml:space="preserve">Generación de tráfico
 </t>
   </si>
   <si>
     <t xml:space="preserve">¿Nutrís de manera sistemática vuestros embudos de ventas mediante tráfico orgánico (no pagado) como la publicidad online (tráfico pagado)?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Tener un embudo de ventas sin tráfico es como tener una farmacia muy bonita en una calle donde NO pasa NADIE.&lt;/b&gt; La parte positiva es que, en el mundo digital, puedes atraer tráfico a tu farmacia.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;incrementar la &lt;i&gt;generación de tráfico&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Tener un embudo de ventas sin tráfico es como tener una farmacia muy bonita en una calle donde NO pasa NADIE.&lt;/b&gt; La parte positiva es que, en el mundo digital, puedes atraer tráfico a tu farmacia.&lt;/p&gt; 
 &lt;p&gt;Un estudio de &lt;i&gt;Neil Patel&lt;/i&gt; revela que el tráfico online puede aumentar las visitas físicas en un 25% si se gestiona adecuadamente.&lt;/p&gt; 
 &lt;p&gt;El tráfico online no solo sirve para vender más a nivel digital, sino también para atraer a más personas a tu farmacia física, por ejemplo, para asistir a una charla o para utilizar vuestros servicios de salud.&lt;/p&gt; 
 &lt;p&gt;El tráfico es &lt;b&gt;savia&lt;/b&gt; que alimenta vuestra farmacia a cualquier nivel.&lt;/p&gt;
@@ -480,18 +484,18 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Crea 10 tipos de mensajes diferentes relacionados con un producto que quieras promover entre tus seguidores e incluye al final de cada uno una llamada a la acción para visiten la página del producto o compren. Intenta que al menos 10 personas accedan al día. &lt;/p&gt; &lt;p&gt;Es decir, no importan los me gusta, sino las acciones que haga relacionada con el producto o servicio que quieras promover. &lt;/p&gt; &lt;p&gt;Esto incrementará el tráfico tanto online como físico, atrayendo a más clientes y potenciando tus oportunidades de ventas. &lt;/p&gt; &lt;p&gt;Una mayor presencia en redes sociales atraerá a más personas a tu farmacia, tanto virtual como físicamente.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;Crea 10 tipos de mensajes diferentes relacionados con un producto que quieras promover entre tus seguidores e incluye al final de cada uno una llamada a la acción para visiten la página del producto o compren. &lt;/p&gt; &lt;p&gt;Intenta que al menos 10 personas accedan al día. &lt;/p&gt; &lt;p&gt;Es decir, no importan los me gusta, sino las acciones que haga relacionada con el producto o servicio que quieras promover. &lt;/p&gt; &lt;p&gt;Esto incrementará el tráfico tanto online como físico, atrayendo a más clientes y potenciando tus oportunidades de ventas. &lt;/p&gt; &lt;p&gt;Una mayor presencia en redes sociales atraerá a más personas a tu farmacia, tanto virtual como físicamente.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;captación automatizada&lt;/i&gt; para tener clientes recurrentes&lt;/b&gt;.&lt;/p&gt;
-</t>
+    <t>Captación automatizada</t>
   </si>
   <si>
     <t xml:space="preserve">¿Tenéis un sistema automatizado que os permita derivar tráfico a los embudos de manera previsible y medible?  </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Si esta es tu necesidad vital, tienes mucho camino recorrido.&lt;/b&gt; Si tienes un embudo con una alta conversión y sabes cómo generar tráfico para nutrirlo, el siguiente paso es &lt;b&gt;AUTOMATIZAR&lt;/b&gt; la captación.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;mejorar la &lt;i&gt;captación automatizada&lt;/i&gt; para tener clientes recurrentes&lt;/b&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Si esta es tu necesidad vital, tienes mucho camino recorrido.&lt;/b&gt; Si tienes un embudo con una alta conversión y sabes cómo generar tráfico para nutrirlo, el siguiente paso es &lt;b&gt;AUTOMATIZAR&lt;/b&gt; la captación.&lt;/p&gt; 
 &lt;p&gt;Un informe de &lt;i&gt;Forrester&lt;/i&gt; indica que las empresas que automatizan sus procesos de captación pueden aumentar sus ingresos en un 40%.&lt;/p&gt; 
 &lt;p&gt;Por ejemplo, si sabes que con 50€ vendes 200€, ¿qué pasaría si invirtieras 200€? ¡Exacto! Ganarías 800€.&lt;/p&gt; 
 &lt;p&gt;Automatizar la captación es un arte, pero es el resultado de todo el trabajo previo que has realizado.&lt;/p&gt;
@@ -499,24 +503,24 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Configura un mensaje automático de bienvenida para nuevos seguidores o suscriptores.&lt;/b&gt; Esto inicia la captación de manera eficiente y asegura que ningún contacto quede desatendido. Según &lt;i&gt;MarketingProfs&lt;/i&gt;, la automatización de mensajes puede mejorar la retención de clientes en un 40%.&lt;/p&gt; &lt;p&gt;Automatizar la captación mejorará la eficiencia y garantizará que los nuevos contactos se mantengan comprometidos desde el inicio.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Configura un mensaje automático de bienvenida para nuevos seguidores o suscriptores.&lt;/b&gt; Esto inicia la captación de manera eficiente y asegura que ningún contacto quede desatendido. &lt;/p&gt; &lt;p&gt;Según &lt;i&gt;MarketingProfs&lt;/i&gt;, la automatización de mensajes puede mejorar la retención de clientes en un 40%.&lt;/p&gt; &lt;p&gt;Automatizar la captación mejorará la eficiencia y garantizará que los nuevos contactos se mantengan comprometidos desde el inicio.&lt;/p&gt;&lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
   <si>
-    <t>&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;desarrollar una &lt;i&gt;visión estratégica&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;</t>
+    <t>Visión estratégica</t>
   </si>
   <si>
     <t>¿Hacéis un seguimiento de los resultados, fijáis objetivos y optimizar el proceso aumentando la competitividad y la rentabilidad?</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;La visión estratégica es lo que os diferenciará y permitirá crecer de manera sostenida.&lt;/b&gt; Según un estudio de &lt;i&gt;BCG&lt;/i&gt;, las empresas con una visión estratégica bien definida tienen un 38% más de probabilidades de tener éxito a largo plazo.&lt;/p&gt; 
+    <t xml:space="preserve">&lt;p&gt;En función de tus respuestas, &lt;b&gt;&lt;i&gt;FarmaCheck&lt;/i&gt;&lt;/b&gt; ha identificado que la Necesidad Vital de la farmacia es &lt;b&gt;desarrollar una &lt;i&gt;visión estratégica&lt;/i&gt;&lt;/b&gt;.&lt;/p&gt;&lt;p&gt;&lt;b&gt;La visión estratégica es lo que os diferenciará y permitirá crecer de manera sostenida.&lt;/b&gt; Según un estudio de &lt;i&gt;BCG&lt;/i&gt;, las empresas con una visión estratégica bien definida tienen un 38% más de probabilidades de tener éxito a largo plazo.&lt;/p&gt; 
 &lt;p&gt;El futuro de la farmacia no está solo en lo que haces ahora, sino en lo que planeas hacer y hacia dónde te diriges.&lt;/p&gt; 
 &lt;p&gt;¡Felicidades por llegar hasta aquí! Ahora toca seguir subiendo y construyendo un futuro sólido para tu farmacia.&lt;/p&gt;
 &lt;p&gt;&lt;i&gt;*Si quieres entender y dominar todo esto, &lt;u&gt;no olvides llegar hasta el final de la página&lt;/u&gt;&lt;/i&gt;.&lt;/p&gt;
 </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige varios indicadores clave que no estés midiendo y empieza a hacerles seguimiento.&lt;/b&gt; Evaluar y analizar datos clave te permitirá tomar decisiones informadas. Un informe de &lt;i&gt;Boston Consulting Group&lt;/i&gt; muestra que las empresas con una visión estratégica clara tienen un 38% más de probabilidad de éxito a largo plazo.&lt;/p&gt; &lt;p&gt;Esto te proporcionará una visión clara del desempeño y permitirá optimizar tus operaciones y estrategias para un crecimiento sostenido.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero NO es suficiente. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás un REGALO que puede marcar la diferencia entre tus farmacias y la competencia. &lt;p&gt;Sigue leyendo.&lt;/p&gt;
+    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;Elige varios indicadores clave que no estés midiendo y empieza a hacerles seguimiento.&lt;/b&gt; &lt;/p&gt; &lt;p&gt;Evaluar y analizar datos clave te permitirá tomar decisiones informadas. Un informe de &lt;i&gt;Boston Consulting Group&lt;/i&gt; muestra que las empresas con una visión estratégica clara tienen un 38% más de probabilidad de éxito a largo plazo.&lt;/p&gt; &lt;p&gt;Esto te proporcionará una visión clara del desempeño y permitirá optimizar tus operaciones y estrategias para un crecimiento sostenido.&lt;/p&gt; &lt;p&gt;Esta es una recomendación sencilla para que puedas empezar a caminar en la dirección correcta, pero &lt;u&gt;NO es suficiente&lt;/u&gt;. &lt;p&gt;Si quieres hacer un cambio &lt;i&gt;realmente notable&lt;/i&gt;, al final de la página encontrarás &lt;b&gt;un REGALO que puede marcar la diferencia entre tus farmacias y la competencia&lt;/b&gt;. &lt;p&gt;
 </t>
   </si>
 </sst>
@@ -821,7 +825,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.63"/>
+    <col customWidth="1" min="1" max="4" width="10.63"/>
+    <col customWidth="1" hidden="1" min="5" max="5" width="10.63"/>
+    <col customWidth="1" min="6" max="26" width="10.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -916,19 +922,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -961,16 +967,16 @@
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1003,16 +1009,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1045,16 +1051,16 @@
         <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -1081,22 +1087,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1123,22 +1129,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1165,22 +1171,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1207,22 +1213,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>31</v>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1249,22 +1255,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1291,22 +1297,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1333,22 +1339,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1375,22 +1381,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>54</v>
+      <c r="D14" s="10" t="s">
+        <v>63</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1417,22 +1423,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>54</v>
+      <c r="D15" s="5" t="s">
+        <v>67</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1459,22 +1465,22 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>54</v>
+      <c r="D16" s="5" t="s">
+        <v>71</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1501,22 +1507,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1543,22 +1549,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>77</v>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1585,22 +1591,22 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>77</v>
+      <c r="D19" s="5" t="s">
+        <v>85</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1627,22 +1633,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>77</v>
+      <c r="D20" s="5" t="s">
+        <v>89</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1669,22 +1675,22 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>77</v>
+      <c r="D21" s="5" t="s">
+        <v>93</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="F21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="G21" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>

</xml_diff>